<commit_message>
update some part number
</commit_message>
<xml_diff>
--- a/Librairies/TEP_243-Altium_RLC_Librairie.xlsx
+++ b/Librairies/TEP_243-Altium_RLC_Librairie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lecegeplimoilou-my.sharepoint.com/personal/kevin_cotton_cegeplimoilou_ca/Documents/_Cours-TGE/Altium/Librairies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1167" documentId="13_ncr:1_{550D3E46-E4B6-4165-A45B-7D583CCE157E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96D158B0-E354-442F-89ED-55B6C5311797}"/>
+  <xr:revisionPtr revIDLastSave="1168" documentId="13_ncr:1_{550D3E46-E4B6-4165-A45B-7D583CCE157E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4544065C-65F4-4103-A394-426AA094816E}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="1044" windowWidth="20772" windowHeight="11580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="384" windowWidth="21180" windowHeight="11736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cap" sheetId="1" r:id="rId1"/>
@@ -1549,7 +1549,7 @@
   <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A23" sqref="A2:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2693,8 +2693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0837104-CD0C-4055-94B3-0A98F94F86E8}">
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A30" sqref="A2:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
add R, simplify ClickBoard Footprint
</commit_message>
<xml_diff>
--- a/Librairies/TEP_243-Altium_RLC_Librairie.xlsx
+++ b/Librairies/TEP_243-Altium_RLC_Librairie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lecegeplimoilou-my.sharepoint.com/personal/kevin_cotton_cegeplimoilou_ca/Documents/_Cours-TGE/Altium/Librairies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lecegeplimoilou-my.sharepoint.com/personal/kevin_cotton_cegeplimoilou_ca/Documents/_Cours-TGE/Altium/243-TEP_Altium-Lib/Librairies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1168" documentId="13_ncr:1_{550D3E46-E4B6-4165-A45B-7D583CCE157E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4544065C-65F4-4103-A394-426AA094816E}"/>
+  <xr:revisionPtr revIDLastSave="1191" documentId="13_ncr:1_{550D3E46-E4B6-4165-A45B-7D583CCE157E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E4F7E99-0171-416A-8546-C9764C6CC03F}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="384" windowWidth="21180" windowHeight="11736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5460" yWindow="1596" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cap" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="389">
   <si>
     <t>Comment</t>
   </si>
@@ -1171,6 +1171,45 @@
   </si>
   <si>
     <t>CAP CER 2.2uF 10V X7R 0603</t>
+  </si>
+  <si>
+    <t>RES030</t>
+  </si>
+  <si>
+    <t>RES031</t>
+  </si>
+  <si>
+    <t>Res 30k 1% 0603</t>
+  </si>
+  <si>
+    <t>Res 150R 1% 0805</t>
+  </si>
+  <si>
+    <t>30k</t>
+  </si>
+  <si>
+    <t>150R</t>
+  </si>
+  <si>
+    <t>RC0805FR-07150RL</t>
+  </si>
+  <si>
+    <t>150V</t>
+  </si>
+  <si>
+    <t>1/8W</t>
+  </si>
+  <si>
+    <t>C114523</t>
+  </si>
+  <si>
+    <t>RC0603FR-0730KL</t>
+  </si>
+  <si>
+    <t>C100001</t>
+  </si>
+  <si>
+    <t>R_2012[0805]</t>
   </si>
 </sst>
 </file>
@@ -1239,7 +1278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1264,6 +1303,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1548,8 +1588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A23" sqref="A2:XFD23"/>
+    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2691,10 +2731,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0837104-CD0C-4055-94B3-0A98F94F86E8}">
-  <dimension ref="A1:S30"/>
+  <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A30" sqref="A2:XFD30"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4202,6 +4242,100 @@
       </c>
       <c r="Q30" t="s">
         <v>359</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>376</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="E31" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" t="s">
+        <v>386</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="I31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J31" t="s">
+        <v>135</v>
+      </c>
+      <c r="K31" t="s">
+        <v>13</v>
+      </c>
+      <c r="L31" t="s">
+        <v>27</v>
+      </c>
+      <c r="M31" t="s">
+        <v>21</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O31" t="s">
+        <v>22</v>
+      </c>
+      <c r="P31" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>377</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="E32" t="s">
+        <v>69</v>
+      </c>
+      <c r="F32" t="s">
+        <v>382</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="I32" t="s">
+        <v>384</v>
+      </c>
+      <c r="J32" t="s">
+        <v>383</v>
+      </c>
+      <c r="K32" t="s">
+        <v>13</v>
+      </c>
+      <c r="L32" t="s">
+        <v>27</v>
+      </c>
+      <c r="M32" t="s">
+        <v>21</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="O32" t="s">
+        <v>22</v>
+      </c>
+      <c r="P32" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>